<commit_message>
Update Rizka - Fixing Data Binding Cari Mobil Lelang
</commit_message>
<xml_diff>
--- a/CariMobilBekasLelang.xlsx
+++ b/CariMobilBekasLelang.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY WORLD\KULIAH (TUGAS)\TGS SEMS. 8\INTERNSHIT\Task ACC ONE\ACC-ACCOne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78A2F7D-05F9-4825-B2FF-6E712AACC54E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B62DEE-E0A8-47FC-AF38-CEF88283C2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="0" windowWidth="17895" windowHeight="11070" xr2:uid="{87F55B32-E5D4-463F-975A-EE0EF98EC384}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{87F55B32-E5D4-463F-975A-EE0EF98EC384}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>lokasi</t>
   </si>
@@ -69,16 +69,26 @@
   </si>
   <si>
     <t>Agya</t>
+  </si>
+  <si>
+    <t>Chery QQ GX 2001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -649,17 +659,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F550555E-CE3F-4AAE-A49C-CF84E091597F}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -698,47 +709,65 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
-        <v>17</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="11">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>9</v>
+      <c r="D3" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
-        <v>15</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
         <v>15</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8">
+        <v>15</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>